<commit_message>
Add TestLogin&Logoff, testClueModify script
</commit_message>
<xml_diff>
--- a/resources/TestContent.xlsx
+++ b/resources/TestContent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestConfiguration" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
   <si>
     <t>XPATH</t>
   </si>
@@ -181,6 +181,66 @@
   </si>
   <si>
     <t>ZunYiMaoTai</t>
+  </si>
+  <si>
+    <t>HomePage_ViewClueOption</t>
+  </si>
+  <si>
+    <t>查看线索</t>
+  </si>
+  <si>
+    <t>VerifyViewCluePage</t>
+  </si>
+  <si>
+    <t>线索工具</t>
+  </si>
+  <si>
+    <t>ViewCluePage_SelectClue1</t>
+  </si>
+  <si>
+    <t>//span[text()='</t>
+  </si>
+  <si>
+    <t>ViewCluePage_SelectClue2</t>
+  </si>
+  <si>
+    <t>']/../../..//a[contains(text(),'修改')]</t>
+  </si>
+  <si>
+    <t>VerifyClueModifyPage</t>
+  </si>
+  <si>
+    <t>编辑线索</t>
+  </si>
+  <si>
+    <t>//textarea[@id='description']</t>
+  </si>
+  <si>
+    <t>ClueModifyPage_TextArea</t>
+  </si>
+  <si>
+    <t>修改线索-修改下次联系时间为当前时间加7天</t>
+  </si>
+  <si>
+    <t>ClueModifyContent</t>
+  </si>
+  <si>
+    <t>//input[@id='nextstep_time']</t>
+  </si>
+  <si>
+    <t>ClueModifyPage_NextTime</t>
+  </si>
+  <si>
+    <t>线索修改成功！</t>
+  </si>
+  <si>
+    <t>VerifyClueMidifyResult</t>
+  </si>
+  <si>
+    <t>//input[@value='返回']</t>
+  </si>
+  <si>
+    <t>ClueModifyPage_SaveBack</t>
   </si>
 </sst>
 </file>
@@ -252,21 +312,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,7 +647,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
@@ -592,19 +655,19 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5"/>
+      <c r="A2" s="6"/>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -612,23 +675,23 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="1"/>
     </row>
   </sheetData>
@@ -642,10 +705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -664,22 +727,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="H1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="4"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -740,6 +803,12 @@
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -793,6 +862,46 @@
       </c>
       <c r="B10" s="1" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -809,29 +918,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.90625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -840,10 +949,10 @@
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -896,13 +1005,25 @@
       <c r="B6" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>50</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -911,6 +1032,20 @@
       </c>
       <c r="B8" t="s">
         <v>49</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add test ClueTransferCustomer Script
</commit_message>
<xml_diff>
--- a/resources/TestContent.xlsx
+++ b/resources/TestContent.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
   <si>
     <t>XPATH</t>
   </si>
@@ -241,6 +241,93 @@
   </si>
   <si>
     <t>ClueModifyPage_SaveBack</t>
+  </si>
+  <si>
+    <t>ViewCluePage_TransferClue1</t>
+  </si>
+  <si>
+    <t>ViewCluePage_TransferClue2</t>
+  </si>
+  <si>
+    <t>']/../../..//a[contains(text(),'转换')]</t>
+  </si>
+  <si>
+    <t>添加客户</t>
+  </si>
+  <si>
+    <t>AddCustomerPage_Name</t>
+  </si>
+  <si>
+    <t>//input[@id='name']</t>
+  </si>
+  <si>
+    <t>AddCustomerPage_Industry</t>
+  </si>
+  <si>
+    <t>//input[@id='industry']</t>
+  </si>
+  <si>
+    <t>AddCustomerPage_ComOrig</t>
+  </si>
+  <si>
+    <t>//select[@id='origin']</t>
+  </si>
+  <si>
+    <t>AddCustomerPage_ComOrigSelection</t>
+  </si>
+  <si>
+    <t>//select[@id='origin']/option[@value='网络营销']</t>
+  </si>
+  <si>
+    <t>AddCustomerPage_ComPro</t>
+  </si>
+  <si>
+    <t>//input[@id='ownership2']</t>
+  </si>
+  <si>
+    <t>//input[@name='con_name']</t>
+  </si>
+  <si>
+    <t>AddCustomerPage_ConName</t>
+  </si>
+  <si>
+    <t>//select[@id='no_of_employees']</t>
+  </si>
+  <si>
+    <t>AddCustomerPage_NumEmp</t>
+  </si>
+  <si>
+    <t>AddCustomerPage_NumEmpSelection</t>
+  </si>
+  <si>
+    <t>//input[@name='create_business2']</t>
+  </si>
+  <si>
+    <t>//select[@id='no_of_employees']/option[@value='5--20人']</t>
+  </si>
+  <si>
+    <t>AddCustomerPage_CreateBussiness</t>
+  </si>
+  <si>
+    <t>//input[@value='保存']</t>
+  </si>
+  <si>
+    <t>AddCustomerPage_SaveBtn</t>
+  </si>
+  <si>
+    <t>添加客户成功</t>
+  </si>
+  <si>
+    <t>VerifyAddCustomerPage</t>
+  </si>
+  <si>
+    <t>VerifyAddCustomerResult</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
+  </si>
+  <si>
+    <t>MaoTaoCEO</t>
   </si>
 </sst>
 </file>
@@ -312,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -322,14 +409,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,7 +735,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
@@ -655,19 +743,19 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -675,23 +763,23 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1"/>
     </row>
   </sheetData>
@@ -705,16 +793,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.1796875" customWidth="1"/>
     <col min="4" max="4" width="29.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
@@ -727,22 +815,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="J1" s="7" t="s">
+      <c r="H1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="7"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -902,6 +990,102 @@
       </c>
       <c r="B15" s="1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -918,29 +1102,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.90625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1044,8 +1228,28 @@
       <c r="A9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>67</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish TestDeleteClue and TestCRM suites
</commit_message>
<xml_diff>
--- a/resources/TestContent.xlsx
+++ b/resources/TestContent.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="113">
   <si>
     <t>XPATH</t>
   </si>
@@ -177,9 +177,6 @@
     <t>VerifyCreateClueResult</t>
   </si>
   <si>
-    <t>茅台镇茅台制酒厂</t>
-  </si>
-  <si>
     <t>ZunYiMaoTai</t>
   </si>
   <si>
@@ -327,7 +324,37 @@
     <t>CustomerName</t>
   </si>
   <si>
-    <t>MaoTaoCEO</t>
+    <t>ViewCluePage_ClueCheckBox1</t>
+  </si>
+  <si>
+    <t>ViewCluePage_ClueCheckBox2</t>
+  </si>
+  <si>
+    <t>']/../../..//input[@class='check_list']</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'批量操作')]</t>
+  </si>
+  <si>
+    <t>ViewCluePage_ClueSelection</t>
+  </si>
+  <si>
+    <t>ViewCluePage_ClueDelete</t>
+  </si>
+  <si>
+    <t>//a[@id='delete']</t>
+  </si>
+  <si>
+    <t>VerifyDeleteClueResult</t>
+  </si>
+  <si>
+    <t>删除成功!</t>
+  </si>
+  <si>
+    <t>贵阳回煞酒厂</t>
+  </si>
+  <si>
+    <t>HuiShaaCEO</t>
   </si>
 </sst>
 </file>
@@ -793,10 +820,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -892,10 +919,10 @@
         <v>9</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -954,138 +981,170 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1102,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1173,7 +1232,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>52</v>
@@ -1187,13 +1246,13 @@
         <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1204,10 +1263,10 @@
         <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1218,38 +1277,46 @@
         <v>49</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add HTMLTestRunner to get html report
</commit_message>
<xml_diff>
--- a/resources/TestContent.xlsx
+++ b/resources/TestContent.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15310" windowHeight="3250" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestConfiguration" sheetId="2" r:id="rId1"/>
     <sheet name="PageElement" sheetId="1" r:id="rId2"/>
     <sheet name="TestData" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A4:J13"/>
 </workbook>
 </file>
 
@@ -177,9 +178,6 @@
     <t>VerifyCreateClueResult</t>
   </si>
   <si>
-    <t>ZunYiMaoTai</t>
-  </si>
-  <si>
     <t>HomePage_ViewClueOption</t>
   </si>
   <si>
@@ -351,17 +349,20 @@
     <t>删除成功!</t>
   </si>
   <si>
-    <t>贵阳回煞酒厂</t>
-  </si>
-  <si>
-    <t>HuiShaaCEO</t>
+    <t>西安长安街科技公司</t>
+  </si>
+  <si>
+    <t>ChangAnKeJi</t>
+  </si>
+  <si>
+    <t>ChangAnKeJiCEO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,6 +381,14 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -423,10 +432,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -438,15 +448,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -752,7 +764,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -762,27 +774,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -790,23 +802,23 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="1"/>
     </row>
   </sheetData>
@@ -814,6 +826,9 @@
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="A5:A9"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -822,7 +837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -842,22 +857,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="E1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="H1" s="10"/>
+      <c r="J1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8"/>
+      <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -919,10 +934,10 @@
         <v>9</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -981,170 +996,170 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1163,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1176,14 +1191,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="8"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1232,7 +1247,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>52</v>
@@ -1246,13 +1261,13 @@
         <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1263,10 +1278,10 @@
         <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1277,46 +1292,46 @@
         <v>49</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>